<commit_message>
Adição de correção deriva instrumental
</commit_message>
<xml_diff>
--- a/GRARED_P_valores.xlsx
+++ b/GRARED_P_valores.xlsx
@@ -519,7 +519,7 @@
   <dimension ref="A1:O12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -695,7 +695,7 @@
         <v>1.89</v>
       </c>
       <c r="L4" s="5">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="M4" s="1">
         <v>12</v>
@@ -739,7 +739,7 @@
         <v>1.4470000000000001</v>
       </c>
       <c r="L5" s="5">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="M5" s="1">
         <v>14</v>
@@ -783,7 +783,7 @@
         <v>1.004</v>
       </c>
       <c r="L6" s="5">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="M6" s="1">
         <v>16</v>
@@ -827,7 +827,7 @@
         <v>0.56100000000000005</v>
       </c>
       <c r="L7" s="5">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="M7" s="1">
         <v>18</v>
@@ -871,7 +871,7 @@
         <v>0.98699999999999999</v>
       </c>
       <c r="L8" s="5">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="M8" s="1">
         <v>20</v>
@@ -915,7 +915,7 @@
         <v>1.413</v>
       </c>
       <c r="L9" s="5">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="M9" s="1">
         <v>22</v>
@@ -959,7 +959,7 @@
         <v>1.839</v>
       </c>
       <c r="L10" s="5">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="M10" s="1">
         <v>24</v>
@@ -1003,7 +1003,7 @@
         <v>2.2650000000000001</v>
       </c>
       <c r="L11" s="5">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="M11" s="1">
         <v>26</v>
@@ -1047,7 +1047,7 @@
         <v>2.3330000000000002</v>
       </c>
       <c r="L12" s="5">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="M12" s="1">
         <v>28</v>

</xml_diff>